<commit_message>
big update fix bug
</commit_message>
<xml_diff>
--- a/TestCaseWeb.xlsx
+++ b/TestCaseWeb.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuxua\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebProgramming_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBAF24F-613E-4BA1-9A5F-3F5E98A76088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11138" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="255" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="97">
   <si>
     <t>Test case description</t>
   </si>
@@ -334,11 +335,17 @@
   <si>
     <t>Home/Setting/Cart (maybe more) has extra "/frontend" in the link</t>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>DOne</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,16 +378,7 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -392,10 +390,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,345 +683,348 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="74" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.3984375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="54.265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="61.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="40.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="26.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5" t="s">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2" t="s">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2" t="s">
+      <c r="G13" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2" t="s">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="3"/>
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+      <c r="D17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2" t="s">
+      <c r="D19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A21" s="3"/>
-      <c r="B21" s="2" t="s">
+      <c r="D20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="3"/>
-      <c r="B22" s="2" t="s">
+      <c r="D21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
+      <c r="D22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="3" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="3"/>
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2" t="s">
+      <c r="D24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="3"/>
-      <c r="B26" s="2" t="s">
+      <c r="D25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="6" t="s">
+      <c r="D26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C28" s="5"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -1044,21 +1054,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1068,8 +1078,11 @@
       <c r="C1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1077,41 +1090,56 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="1"/>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="1"/>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="1" t="s">
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="1"/>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
       <c r="C7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1119,52 +1147,70 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>94</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add testcase and new sql script
</commit_message>
<xml_diff>
--- a/TestCaseWeb.xlsx
+++ b/TestCaseWeb.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebProgramming_Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\webassignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBAF24F-613E-4BA1-9A5F-3F5E98A76088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="255" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="258" windowWidth="28800" windowHeight="15558"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="120">
   <si>
     <t>Test case description</t>
   </si>
@@ -341,11 +340,80 @@
   <si>
     <t>DOne</t>
   </si>
+  <si>
+    <t>Test logout when cart have item</t>
+  </si>
+  <si>
+    <t>Cart still have item</t>
+  </si>
+  <si>
+    <t>Readd an item into cart</t>
+  </si>
+  <si>
+    <t>Warning pop up</t>
+  </si>
+  <si>
+    <t>See newly added user</t>
+  </si>
+  <si>
+    <t>See error and can not add</t>
+  </si>
+  <si>
+    <t>See newly updated information</t>
+  </si>
+  <si>
+    <t>See error and can not update user</t>
+  </si>
+  <si>
+    <t>Admin add user</t>
+  </si>
+  <si>
+    <t>Admin add user empty field</t>
+  </si>
+  <si>
+    <t>Admin update user information</t>
+  </si>
+  <si>
+    <t>Admin update user empty field</t>
+  </si>
+  <si>
+    <t>Staff/Admin add product</t>
+  </si>
+  <si>
+    <t>See newly added product</t>
+  </si>
+  <si>
+    <t>Staff/Admin add product missing fields</t>
+  </si>
+  <si>
+    <t>See error and can not add new product</t>
+  </si>
+  <si>
+    <t>Staff/Admin update product information</t>
+  </si>
+  <si>
+    <t>See error and can not update product</t>
+  </si>
+  <si>
+    <t>Staff/Admin update product image</t>
+  </si>
+  <si>
+    <t>See newly updated product image</t>
+  </si>
+  <si>
+    <t>Staff/Admin update wrong/empty image file</t>
+  </si>
+  <si>
+    <t>Cannot update</t>
+  </si>
+  <si>
+    <t>View category, sort, filter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -390,10 +458,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -683,25 +754,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="74" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.41796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="54.26171875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.41796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="40.15625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -721,7 +792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -731,14 +802,14 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -746,15 +817,15 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>4</v>
@@ -764,7 +835,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="2" t="s">
@@ -772,7 +843,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -782,30 +853,30 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
@@ -815,7 +886,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -827,7 +898,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -841,7 +912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
@@ -851,7 +922,7 @@
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>60</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -861,7 +932,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -871,7 +942,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6"/>
       <c r="B15" s="1" t="s">
         <v>43</v>
@@ -881,7 +952,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
@@ -891,14 +962,14 @@
       <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6"/>
       <c r="B17" s="1" t="s">
         <v>59</v>
@@ -909,7 +980,7 @@
       <c r="D17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
@@ -926,7 +997,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6"/>
       <c r="B19" s="1" t="s">
         <v>68</v>
@@ -937,7 +1008,7 @@
       <c r="D19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6"/>
       <c r="B20" s="1" t="s">
         <v>71</v>
@@ -948,7 +1019,7 @@
       <c r="D20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6"/>
       <c r="B21" s="1" t="s">
         <v>73</v>
@@ -959,7 +1030,7 @@
       <c r="D21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
         <v>75</v>
@@ -970,7 +1041,7 @@
       <c r="D22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>79</v>
       </c>
@@ -985,7 +1056,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
         <v>81</v>
@@ -993,7 +1064,7 @@
       <c r="D24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>82</v>
@@ -1001,7 +1072,7 @@
       <c r="D25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6"/>
       <c r="B26" s="1" t="s">
         <v>83</v>
@@ -1009,7 +1080,7 @@
       <c r="D26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
@@ -1023,11 +1094,123 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="5"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="D8:D10"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="F23:F26"/>
@@ -1040,13 +1223,6 @@
     <mergeCell ref="F18:F22"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1054,21 +1230,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1082,7 +1258,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1090,8 +1266,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
@@ -1101,8 +1277,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -1110,8 +1286,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>41</v>
       </c>
@@ -1119,8 +1295,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C6" t="s">
@@ -1130,8 +1306,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="10"/>
       <c r="C7" t="s">
         <v>47</v>
       </c>
@@ -1139,7 +1315,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1147,7 +1323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1158,7 +1334,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1169,7 +1345,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1180,7 +1356,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1191,7 +1367,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1202,7 +1378,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Test case file updates.
</commit_message>
<xml_diff>
--- a/TestCaseWeb.xlsx
+++ b/TestCaseWeb.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="159">
   <si>
     <t>Test case description</t>
   </si>
@@ -298,18 +298,6 @@
     <t>DOne</t>
   </si>
   <si>
-    <t>See newly added user</t>
-  </si>
-  <si>
-    <t>See error and can not add</t>
-  </si>
-  <si>
-    <t>See newly updated information</t>
-  </si>
-  <si>
-    <t>See error and can not update user</t>
-  </si>
-  <si>
     <t>Admin add user</t>
   </si>
   <si>
@@ -350,10 +338,6 @@
   </si>
   <si>
     <t>Discount doesn’t apply</t>
-  </si>
-  <si>
-    <t>How to reproduce: Change Deactivate product to YES &gt; Go to homepage &gt; Change product.
-Bug: The Deactivate status displays NO. If continue changing, the status NO is applied.</t>
   </si>
   <si>
     <t>Add button in "Add new product" modal doesn't work</t>
@@ -433,9 +417,6 @@
   </si>
   <si>
     <t>Product information is updated</t>
-  </si>
-  <si>
-    <t>Correct inputs but wrong popup (red warning) show up</t>
   </si>
   <si>
     <t>Setting/Password</t>
@@ -520,6 +501,44 @@
   </si>
   <si>
     <t>At login page, click on "Go to register" button</t>
+  </si>
+  <si>
+    <t>How to reproduce: Change Deactivate product to YES &gt; Go to homepage (Or reload) &gt; Change product.
+Bug: The Deactivate status displays NO. If continue changing, the status NO is applied.</t>
+  </si>
+  <si>
+    <t>On each user, click Update button</t>
+  </si>
+  <si>
+    <t>All forms filled out: nothing happens.
+Form is empty or in wrong format: waring on each form.</t>
+  </si>
+  <si>
+    <t>Changes applied.
+Database updated.</t>
+  </si>
+  <si>
+    <t>Modal is closed.
+No change applied. Previous changes are reset.</t>
+  </si>
+  <si>
+    <t>User information is updated</t>
+  </si>
+  <si>
+    <t>In Manage user page, click Add button</t>
+  </si>
+  <si>
+    <t>Database updated.</t>
+  </si>
+  <si>
+    <t>New user registered to the database.</t>
+  </si>
+  <si>
+    <t>Is ok to ignore this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct inputs but clicking update button doesn’t show any success message.
+Forms should reset value afterwards. </t>
   </si>
 </sst>
 </file>
@@ -555,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -579,10 +598,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -592,12 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,15 +646,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>757238</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>50062</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>252413</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>131025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -646,7 +671,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4910139" y="4705351"/>
+          <a:off x="5619751" y="5510214"/>
           <a:ext cx="3362325" cy="2040786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -924,9 +949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -961,117 +986,117 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>131</v>
+      <c r="E2" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="8"/>
-      <c r="B3" s="14" t="s">
-        <v>112</v>
+      <c r="A3" s="10"/>
+      <c r="B3" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="8"/>
-      <c r="B4" s="14"/>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="13"/>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>131</v>
+      <c r="E8" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1081,12 +1106,12 @@
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="8"/>
+      <c r="C11" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="10"/>
       <c r="E11" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -1098,18 +1123,18 @@
         <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="96" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1118,70 +1143,70 @@
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>131</v>
+      <c r="E13" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="8"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+        <v>126</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D16" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="8"/>
+      <c r="E16" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1190,111 +1215,113 @@
       <c r="C18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="8"/>
+      <c r="E18" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="8"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="8"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A21" s="8"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+        <v>128</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="8"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="E23" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="8"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+        <v>129</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="8"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+        <v>131</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="8"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+        <v>130</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
@@ -1303,294 +1330,352 @@
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="A28" s="10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="8"/>
+      <c r="B28" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A29" s="10"/>
+      <c r="B29" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="8"/>
-      <c r="D30" s="3" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="10"/>
+      <c r="B31" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="B32" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="10"/>
+      <c r="B33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="10"/>
+      <c r="B34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="10"/>
+      <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="8"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="8"/>
-      <c r="D34" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="8" t="s">
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="4" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="8"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="8"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A39" s="10"/>
+      <c r="B39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A40" s="10"/>
+      <c r="B40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="10"/>
+      <c r="B41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="8"/>
-      <c r="B39" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A40" s="8"/>
-      <c r="B40" s="1" t="s">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="10"/>
+      <c r="B43" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="8"/>
-      <c r="B41" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="8"/>
-      <c r="B43" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="8"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="8"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="F44" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A45" s="10"/>
+      <c r="B45" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="10"/>
+      <c r="B46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="F46" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="10"/>
+      <c r="B47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="10"/>
+      <c r="B48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="F44" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="8"/>
-      <c r="B45" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A46" s="8"/>
-      <c r="B46" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" s="8"/>
-      <c r="F46" s="5" t="s">
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="8"/>
-      <c r="B47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D47" s="8"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A48" s="8"/>
-      <c r="B48" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="8" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="10"/>
+      <c r="B50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="10"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="10"/>
+      <c r="B51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="10"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="10"/>
+      <c r="B52" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="8"/>
-      <c r="B50" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="8"/>
-      <c r="B51" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="8"/>
-      <c r="B52" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="8"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D53" s="8"/>
+        <v>138</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="8"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D54" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="8"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A49:A55"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E36:E41"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="D42:D48"/>
-    <mergeCell ref="E2:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="D23:D26"/>
+  <mergeCells count="43">
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="D32:D35"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="D13:D15"/>
@@ -1602,17 +1687,29 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E36:E41"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="D42:D48"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="D23:D26"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="D2:D7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="D36:D41"/>
-    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A49:A55"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1623,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1657,7 +1754,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B3" t="s">
@@ -1668,7 +1765,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1677,7 +1774,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -1686,7 +1783,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
@@ -1697,7 +1794,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B7" s="12"/>
+      <c r="B7" s="16"/>
       <c r="C7" t="s">
         <v>41</v>
       </c>
@@ -1712,6 +1809,9 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
@@ -1781,50 +1881,53 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>104</v>
+        <v>148</v>
+      </c>
+      <c r="E20" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
@@ -1832,7 +1935,7 @@
         <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -1840,26 +1943,26 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" t="s">
-        <v>129</v>
+        <v>124</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>